<commit_message>
[Feat : KSW] Add Monster Table, DataManager SingleTon
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\TheLegendoftheArcher_8team\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F57ACE1E-A3D3-438A-B9EF-7F128A09BC48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEE42B5-1C57-40B7-942C-8930E827443F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11700" xr2:uid="{EF0ED782-F235-4F95-9FBE-1C2D9F88973A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Grade</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,6 +48,14 @@
   </si>
   <si>
     <t>Artifact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MonsterGrade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,13 +420,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059B7114-4FA0-43F1-B3D1-3369D94A76BB}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -440,8 +451,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "[Feat : KSW] Add Monster Table, DataManager SingleTon"
This reverts commit f67e20a4edc807e4eae90bf275f17a32b2ad24a0.
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\TheLegendoftheArcher_8team\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEE42B5-1C57-40B7-942C-8930E827443F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F57ACE1E-A3D3-438A-B9EF-7F128A09BC48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11700" xr2:uid="{EF0ED782-F235-4F95-9FBE-1C2D9F88973A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Grade</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,14 +48,6 @@
   </si>
   <si>
     <t>Artifact</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MonsterGrade</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -420,16 +412,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059B7114-4FA0-43F1-B3D1-3369D94A76BB}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -451,20 +440,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Feat : KSW] Fix AbilityTable Component
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\TheLegendoftheArcher_8team\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEE42B5-1C57-40B7-942C-8930E827443F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0465FC4F-3DE3-412B-B760-4B06B8FE10FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11700" xr2:uid="{EF0ED782-F235-4F95-9FBE-1C2D9F88973A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Grade</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,6 +57,34 @@
   <si>
     <t>Boss</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DamageUp</t>
+  </si>
+  <si>
+    <t>AttackSpeedUp</t>
+  </si>
+  <si>
+    <t>MoveSpeedUp</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>HeadShot</t>
+  </si>
+  <si>
+    <t>Evasion</t>
+  </si>
+  <si>
+    <t>ExtraProjectile</t>
   </si>
 </sst>
 </file>
@@ -420,18 +448,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059B7114-4FA0-43F1-B3D1-3369D94A76BB}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -460,6 +496,35 @@
       </c>
       <c r="C2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>